<commit_message>
Changes of 23rd March 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CrudOperation.xlsx
+++ b/FedExApplication/src/TestFiles/CrudOperation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
   <si>
     <t>Nothing Bundt Cakes</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>320018032980</t>
+  </si>
+  <si>
+    <t>320018099707</t>
+  </si>
+  <si>
+    <t>320018099718</t>
+  </si>
+  <si>
+    <t>320018099740</t>
+  </si>
+  <si>
+    <t>320018110017</t>
   </si>
 </sst>
 </file>
@@ -627,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
@@ -753,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="Q2" t="s">
         <v>55</v>
@@ -806,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
         <v>56</v>
@@ -859,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Changes of 28th March 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CrudOperation.xlsx
+++ b/FedExApplication/src/TestFiles/CrudOperation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="67">
   <si>
     <t>Nothing Bundt Cakes</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>320018114229</t>
+  </si>
+  <si>
+    <t>320018117960</t>
   </si>
 </sst>
 </file>
@@ -768,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
         <v>55</v>

</xml_diff>